<commit_message>
resume extractor additional property script
</commit_message>
<xml_diff>
--- a/input_data/resume_extractor_sheet/resume_extractor_additional_prop_input_sheet.xlsx
+++ b/input_data/resume_extractor_sheet/resume_extractor_additional_prop_input_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">FileName</t>
   </si>
@@ -156,6 +156,104 @@
         "toMonth": "10",
         "toYear": "2022",
         "IsLatest": 0
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thriveni.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "college": "KITS College, Kodad, Telangana",
+        "degree": "B.Tech",
+        "branch": "",
+        "yop": "",
+        "cgpa/%": "",
+        "isFinal": 0
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "company": "UI Sottech Pvt Ltd",
+        "designation": "",
+        "fromMonth": "07",
+        "fromYear": "2022",
+        "toMonth": "07",
+        "toYear": "2024",
+        "IsLatest": 1
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vipin_yadav_cv.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/07/2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "college": "Thakur tej Bahadur institute of technology karampur saidpur Ghazipur",
+        "degree": "Diploma",
+        "branch": "Electrical Engineering",
+        "yop": "2020",
+        "cgpa/%": "",
+        "isFinal": 1
+    },
+    {
+        "college": "Up Board",
+        "degree": "12th",
+        "branch": "",
+        "yop": "2017",
+        "cgpa/%": "79",
+        "isFinal": 0
+    },
+    {
+        "college": "Up board",
+        "degree": "10th",
+        "branch": "",
+        "yop": "2015",
+        "cgpa/%": "83",
+        "isFinal": 0
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "company": "Samvdhana Motherson internation ltd.",
+        "designation": "Assistant Engineer",
+        "fromMonth": "06",
+        "fromYear": "2022",
+        "toMonth": "06",
+        "toYear": "25",
+        "IsLatest": 1
+    }
+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ArreeshRajan.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[
+    {
+        "college": "",
+        "degree": "Executive MBA",
+        "branch": "",
+        "yop": "",
+        "cgpa/%": "",
+        "isFinal": 0
+    },
+    {
+        "college": "",
+        "degree": "B.Tech",
+        "branch": "Information Technology",
+        "yop": "",
+        "cgpa/%": "",
+        "isFinal": 0
     }
 ]</t>
   </si>
@@ -343,10 +441,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,7 +461,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="48.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="51.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -435,6 +535,57 @@
       </c>
       <c r="K3" s="4" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="127.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="299.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="207.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>